<commit_message>
-- sight was renamed to vision -- position was renamed to stance -- csv-file was created
</commit_message>
<xml_diff>
--- a/NEX2018_08/Project/Data/experimental_data_raw.xlsx
+++ b/NEX2018_08/Project/Data/experimental_data_raw.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\belov\OneDrive - Merck Sharp &amp; Dohme, Corp\Documents\git-repositories\NEX\NEX2018_08\Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{67D61364-BD45-410C-BCB1-5393E5F818EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6E1DA928-D7BE-45FF-9C35-95F99BEC3A38}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{4F67C8B8-6913-4385-AB8B-C5BD7238E483}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>filling</t>
   </si>
   <si>
-    <t>sight</t>
+    <t>measurement</t>
   </si>
   <si>
-    <t>position</t>
+    <t>vision</t>
   </si>
   <si>
-    <t>measurement</t>
+    <t>stance</t>
   </si>
 </sst>
 </file>
@@ -399,8 +399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26F50E29-73F4-4137-BBBA-96DF4F844F9B}">
   <dimension ref="A1:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="I75" sqref="I75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,13 +419,13 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2281,7 +2281,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0D699992-4B4E-487D-A12C-1F79C826B7D4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3EF406-04ED-4478-9A81-33D7675B10EC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>

</xml_diff>